<commit_message>
update initial pieces and placements
</commit_message>
<xml_diff>
--- a/misc/initial-placements-layout.xlsx
+++ b/misc/initial-placements-layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\games-of-the-general\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1AD766-5695-4483-AB7C-56A868781CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA81923C-2F38-4384-84B9-CB1543176350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3800" yWindow="3800" windowWidth="28800" windowHeight="15370" xr2:uid="{9E148E71-0F64-463C-8D1F-6DE2F8F2E947}"/>
   </bookViews>
@@ -104,13 +104,13 @@
     <t>MAJ</t>
   </si>
   <si>
-    <t>CAP</t>
-  </si>
-  <si>
     <t>1LT</t>
   </si>
   <si>
     <t>2LT</t>
+  </si>
+  <si>
+    <t>CPT</t>
   </si>
 </sst>
 </file>
@@ -499,7 +499,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -567,10 +567,10 @@
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>18</v>
@@ -591,7 +591,7 @@
         <v>21</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K3" s="1">
         <v>8</v>
@@ -723,10 +723,10 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>18</v>
@@ -747,7 +747,7 @@
         <v>21</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K9" s="1">
         <v>2</v>

</xml_diff>

<commit_message>
set piece images; rearrange piece image locations
</commit_message>
<xml_diff>
--- a/misc/initial-placements-layout.xlsx
+++ b/misc/initial-placements-layout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\games-of-the-general\misc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Projects\react-tutorial\games-of-the-general\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA81923C-2F38-4384-84B9-CB1543176350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D68467-E250-4DAC-88E0-EDA8DE35D566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3800" yWindow="3800" windowWidth="28800" windowHeight="15370" xr2:uid="{9E148E71-0F64-463C-8D1F-6DE2F8F2E947}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{9E148E71-0F64-463C-8D1F-6DE2F8F2E947}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -200,9 +200,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -240,7 +240,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -346,7 +346,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -488,7 +488,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -496,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{776EF70E-3896-4419-B45B-5BE9A303E1D6}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -541,7 +541,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -559,12 +559,12 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>22</v>
@@ -594,12 +594,12 @@
         <v>23</v>
       </c>
       <c r="K3" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>14</v>
@@ -629,12 +629,12 @@
         <v>14</v>
       </c>
       <c r="K4" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -646,12 +646,12 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -663,150 +663,133 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="K7" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="K8" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K9" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="1">
-        <v>1</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="E10" s="1" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>